<commit_message>
Upload fixed data.json and report-checklist.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111NUVIA1/NUVIA/VAIDOC/4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111NUVIA1/NUVIA/VAIDOC/4.0/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nuvia/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nuvia/Projects/fse/invio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0879B7B3-EC5E-A64D-A910-A64AA0ACB2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F898A3D-868C-A147-82C4-2BDE37EDA78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="500" windowWidth="40220" windowHeight="22540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40960" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -962,28 +962,10 @@
     <t>subject_application_id: VAIDOC</t>
   </si>
   <si>
-    <t>0ba602bf135339bb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.955a9cc12b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-09-23T14:01:02Z</t>
-  </si>
-  <si>
     <t>Non obbligatorio in ottemperanza a quanto espresso dal Decreto settembre 2023</t>
   </si>
   <si>
     <t>Non obbligatorio in ottemperanza a quanto espresso dal Decreto 7 settembre 2023</t>
-  </si>
-  <si>
-    <t>6b51c3e5ffcec1b8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.6057ec4ba2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-09-23T14:46:01Z</t>
   </si>
   <si>
     <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
@@ -991,19 +973,37 @@
 </t>
   </si>
   <si>
-    <t>2025-09-24T10:35:42Z</t>
-  </si>
-  <si>
-    <t>cc58584ae05f7c05</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.97bb3fc5bee3032679f4f07419e04af6375baafa17024527a98ede920c6812ed.d12325dfb1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Errore gestito dall'operatore di backoffice. Il documento sarà collocato nuovamente nella coda di invio a FSE</t>
   </si>
   <si>
     <t>Connection Timeout</t>
+  </si>
+  <si>
+    <t>2025-10-09T14:15:49Z</t>
+  </si>
+  <si>
+    <t>b1106d0b6654ef23</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.f08192632027d5956ed6a07d68b06d48f6dae1379c77abcb01ca7abb3201bccf.41c4666ee5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-10-09T14:17:27Z</t>
+  </si>
+  <si>
+    <t>2e27c382317b1830</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.45e41916eccfe7d335bdfda08434a77f80f5a2e65e09f4d5dde28140bce793d7.1c5704c8e9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-10-09T14:06:19Z</t>
+  </si>
+  <si>
+    <t>72ea4561371f31ea</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.1035347294^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3125,10 +3125,10 @@
   <dimension ref="A1:W632"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="D68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="O19" sqref="O19"/>
+      <selection pane="bottomRight" activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3442,7 +3442,7 @@
         <v>128</v>
       </c>
       <c r="L10" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M10" s="38"/>
       <c r="N10" s="38"/>
@@ -3485,7 +3485,7 @@
         <v>128</v>
       </c>
       <c r="L11" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M11" s="38"/>
       <c r="N11" s="38"/>
@@ -3528,7 +3528,7 @@
         <v>128</v>
       </c>
       <c r="L12" s="38" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M12" s="38"/>
       <c r="N12" s="38"/>
@@ -3571,7 +3571,7 @@
         <v>128</v>
       </c>
       <c r="L13" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M13" s="38"/>
       <c r="N13" s="38"/>
@@ -3614,7 +3614,7 @@
         <v>128</v>
       </c>
       <c r="L14" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M14" s="38"/>
       <c r="N14" s="38"/>
@@ -3657,7 +3657,7 @@
         <v>128</v>
       </c>
       <c r="L15" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M15" s="38"/>
       <c r="N15" s="38"/>
@@ -3700,7 +3700,7 @@
         <v>128</v>
       </c>
       <c r="L16" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M16" s="38"/>
       <c r="N16" s="38"/>
@@ -3748,7 +3748,7 @@
         <v>54</v>
       </c>
       <c r="O17" s="38" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="P17" s="38" t="s">
         <v>54</v>
@@ -3760,7 +3760,7 @@
         <v>54</v>
       </c>
       <c r="S17" s="54" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="T17" s="38"/>
       <c r="U17" s="39" t="s">
@@ -3803,7 +3803,7 @@
         <v>54</v>
       </c>
       <c r="O18" s="38" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="P18" s="38" t="s">
         <v>54</v>
@@ -3815,7 +3815,7 @@
         <v>54</v>
       </c>
       <c r="S18" s="54" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="T18" s="38"/>
       <c r="U18" s="39" t="s">
@@ -3858,7 +3858,7 @@
         <v>54</v>
       </c>
       <c r="O19" s="38" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="P19" s="38" t="s">
         <v>54</v>
@@ -3870,7 +3870,7 @@
         <v>54</v>
       </c>
       <c r="S19" s="54" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="T19" s="38"/>
       <c r="U19" s="39" t="s">
@@ -3908,7 +3908,7 @@
         <v>128</v>
       </c>
       <c r="L20" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M20" s="38"/>
       <c r="N20" s="38"/>
@@ -3951,7 +3951,7 @@
         <v>128</v>
       </c>
       <c r="L21" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M21" s="38"/>
       <c r="N21" s="38"/>
@@ -3994,7 +3994,7 @@
         <v>128</v>
       </c>
       <c r="L22" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M22" s="38"/>
       <c r="N22" s="38"/>
@@ -4037,7 +4037,7 @@
         <v>128</v>
       </c>
       <c r="L23" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M23" s="38"/>
       <c r="N23" s="38"/>
@@ -4080,7 +4080,7 @@
         <v>128</v>
       </c>
       <c r="L24" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M24" s="38"/>
       <c r="N24" s="38"/>
@@ -4123,7 +4123,7 @@
         <v>128</v>
       </c>
       <c r="L25" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M25" s="38"/>
       <c r="N25" s="38"/>
@@ -4166,7 +4166,7 @@
         <v>128</v>
       </c>
       <c r="L26" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M26" s="38"/>
       <c r="N26" s="38"/>
@@ -4209,7 +4209,7 @@
         <v>128</v>
       </c>
       <c r="L27" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M27" s="38"/>
       <c r="N27" s="38"/>
@@ -4252,7 +4252,7 @@
         <v>128</v>
       </c>
       <c r="L28" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M28" s="38"/>
       <c r="N28" s="38"/>
@@ -4295,7 +4295,7 @@
         <v>128</v>
       </c>
       <c r="L29" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M29" s="38"/>
       <c r="N29" s="38"/>
@@ -4338,7 +4338,7 @@
         <v>128</v>
       </c>
       <c r="L30" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M30" s="38"/>
       <c r="N30" s="38"/>
@@ -4381,7 +4381,7 @@
         <v>128</v>
       </c>
       <c r="L31" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M31" s="38"/>
       <c r="N31" s="38"/>
@@ -4424,7 +4424,7 @@
         <v>128</v>
       </c>
       <c r="L32" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M32" s="38"/>
       <c r="N32" s="38"/>
@@ -4467,7 +4467,7 @@
         <v>128</v>
       </c>
       <c r="L33" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M33" s="38"/>
       <c r="N33" s="38"/>
@@ -4510,7 +4510,7 @@
         <v>128</v>
       </c>
       <c r="L34" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M34" s="38"/>
       <c r="N34" s="38"/>
@@ -4553,7 +4553,7 @@
         <v>128</v>
       </c>
       <c r="L35" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M35" s="38"/>
       <c r="N35" s="38"/>
@@ -4596,7 +4596,7 @@
         <v>128</v>
       </c>
       <c r="L36" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M36" s="38"/>
       <c r="N36" s="38"/>
@@ -4639,7 +4639,7 @@
         <v>128</v>
       </c>
       <c r="L37" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M37" s="38"/>
       <c r="N37" s="38"/>
@@ -4682,7 +4682,7 @@
         <v>128</v>
       </c>
       <c r="L38" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M38" s="38"/>
       <c r="N38" s="38"/>
@@ -4725,7 +4725,7 @@
         <v>128</v>
       </c>
       <c r="L39" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M39" s="38"/>
       <c r="N39" s="38"/>
@@ -4768,7 +4768,7 @@
         <v>128</v>
       </c>
       <c r="L40" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M40" s="38"/>
       <c r="N40" s="38"/>
@@ -4811,7 +4811,7 @@
         <v>128</v>
       </c>
       <c r="L41" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M41" s="38"/>
       <c r="N41" s="38"/>
@@ -4854,7 +4854,7 @@
         <v>128</v>
       </c>
       <c r="L42" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M42" s="38"/>
       <c r="N42" s="38"/>
@@ -4897,7 +4897,7 @@
         <v>128</v>
       </c>
       <c r="L43" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M43" s="38"/>
       <c r="N43" s="38"/>
@@ -4940,7 +4940,7 @@
         <v>128</v>
       </c>
       <c r="L44" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M44" s="38"/>
       <c r="N44" s="38"/>
@@ -4983,7 +4983,7 @@
         <v>128</v>
       </c>
       <c r="L45" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M45" s="38"/>
       <c r="N45" s="38"/>
@@ -5026,7 +5026,7 @@
         <v>128</v>
       </c>
       <c r="L46" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M46" s="38"/>
       <c r="N46" s="38"/>
@@ -5069,7 +5069,7 @@
         <v>128</v>
       </c>
       <c r="L47" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M47" s="38"/>
       <c r="N47" s="38"/>
@@ -5112,7 +5112,7 @@
         <v>128</v>
       </c>
       <c r="L48" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M48" s="38"/>
       <c r="N48" s="38"/>
@@ -5155,7 +5155,7 @@
         <v>128</v>
       </c>
       <c r="L49" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M49" s="38"/>
       <c r="N49" s="38"/>
@@ -5198,7 +5198,7 @@
         <v>128</v>
       </c>
       <c r="L50" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M50" s="38"/>
       <c r="N50" s="38"/>
@@ -5241,7 +5241,7 @@
         <v>128</v>
       </c>
       <c r="L51" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M51" s="38"/>
       <c r="N51" s="38"/>
@@ -5284,7 +5284,7 @@
         <v>128</v>
       </c>
       <c r="L52" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M52" s="38"/>
       <c r="N52" s="38"/>
@@ -5327,7 +5327,7 @@
         <v>128</v>
       </c>
       <c r="L53" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M53" s="38"/>
       <c r="N53" s="38"/>
@@ -5370,7 +5370,7 @@
         <v>128</v>
       </c>
       <c r="L54" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M54" s="38"/>
       <c r="N54" s="38"/>
@@ -5413,7 +5413,7 @@
         <v>128</v>
       </c>
       <c r="L55" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M55" s="38"/>
       <c r="N55" s="38"/>
@@ -5456,7 +5456,7 @@
         <v>128</v>
       </c>
       <c r="L56" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M56" s="38"/>
       <c r="N56" s="38"/>
@@ -5499,7 +5499,7 @@
         <v>128</v>
       </c>
       <c r="L57" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M57" s="38"/>
       <c r="N57" s="38"/>
@@ -5542,7 +5542,7 @@
         <v>128</v>
       </c>
       <c r="L58" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M58" s="38"/>
       <c r="N58" s="38"/>
@@ -5585,7 +5585,7 @@
         <v>128</v>
       </c>
       <c r="L59" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M59" s="38"/>
       <c r="N59" s="38"/>
@@ -5628,7 +5628,7 @@
         <v>128</v>
       </c>
       <c r="L60" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M60" s="38"/>
       <c r="N60" s="38"/>
@@ -5661,16 +5661,16 @@
         <v>173</v>
       </c>
       <c r="F61" s="48">
-        <v>45923</v>
+        <v>45939</v>
       </c>
       <c r="G61" s="48" t="s">
+        <v>222</v>
+      </c>
+      <c r="H61" s="48" t="s">
+        <v>223</v>
+      </c>
+      <c r="I61" s="49" t="s">
         <v>224</v>
-      </c>
-      <c r="H61" s="48" t="s">
-        <v>222</v>
-      </c>
-      <c r="I61" s="49" t="s">
-        <v>223</v>
       </c>
       <c r="J61" s="50" t="s">
         <v>54</v>
@@ -5718,7 +5718,7 @@
         <v>128</v>
       </c>
       <c r="L62" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M62" s="38"/>
       <c r="N62" s="38"/>
@@ -5748,19 +5748,19 @@
         <v>168</v>
       </c>
       <c r="E63" s="47" t="s">
+        <v>219</v>
+      </c>
+      <c r="F63" s="48">
+        <v>45939</v>
+      </c>
+      <c r="G63" s="48" t="s">
         <v>225</v>
       </c>
-      <c r="F63" s="48">
-        <v>45924</v>
-      </c>
-      <c r="G63" s="48" t="s">
+      <c r="H63" s="48" t="s">
         <v>226</v>
       </c>
-      <c r="H63" s="48" t="s">
+      <c r="I63" s="49" t="s">
         <v>227</v>
-      </c>
-      <c r="I63" s="49" t="s">
-        <v>228</v>
       </c>
       <c r="J63" s="50" t="s">
         <v>54</v>
@@ -5808,7 +5808,7 @@
         <v>128</v>
       </c>
       <c r="L64" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M64" s="38"/>
       <c r="N64" s="38"/>
@@ -5851,7 +5851,7 @@
         <v>128</v>
       </c>
       <c r="L65" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M65" s="38"/>
       <c r="N65" s="38"/>
@@ -5894,7 +5894,7 @@
         <v>128</v>
       </c>
       <c r="L66" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M66" s="38"/>
       <c r="N66" s="38"/>
@@ -5937,7 +5937,7 @@
         <v>128</v>
       </c>
       <c r="L67" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M67" s="38"/>
       <c r="N67" s="38"/>
@@ -5970,16 +5970,16 @@
         <v>192</v>
       </c>
       <c r="F68" s="48">
-        <v>45923</v>
+        <v>45939</v>
       </c>
       <c r="G68" s="48" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="H68" s="48" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="I68" s="49" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="J68" s="50" t="s">
         <v>54</v>
@@ -6027,7 +6027,7 @@
         <v>128</v>
       </c>
       <c r="L69" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M69" s="38"/>
       <c r="N69" s="38"/>
@@ -6070,7 +6070,7 @@
         <v>128</v>
       </c>
       <c r="L70" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M70" s="38"/>
       <c r="N70" s="38"/>
@@ -6113,7 +6113,7 @@
         <v>128</v>
       </c>
       <c r="L71" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M71" s="38"/>
       <c r="N71" s="38"/>
@@ -6156,7 +6156,7 @@
         <v>128</v>
       </c>
       <c r="L72" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M72" s="38"/>
       <c r="N72" s="38"/>
@@ -12473,6 +12473,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -12730,18 +12742,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -12752,6 +12752,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12770,23 +12787,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>

</xml_diff>